<commit_message>
added sql query to create DB
</commit_message>
<xml_diff>
--- a/excel_files/Clean_Stock_Data.xlsx
+++ b/excel_files/Clean_Stock_Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,19 +545,19 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8.890000000000001</v>
+        <v>8.74</v>
       </c>
       <c r="E4" t="n">
-        <v>8.890000000000001</v>
+        <v>8.77</v>
       </c>
       <c r="F4" t="n">
         <v>0.536475</v>
       </c>
       <c r="G4" t="n">
-        <v>9.071999999999999</v>
+        <v>8.914999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>13645617152</v>
+        <v>13480837120</v>
       </c>
     </row>
     <row r="5">
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
       <c r="E5" t="n">
-        <v>4.4</v>
+        <v>4.35</v>
       </c>
       <c r="F5" t="n">
         <v>0.168911</v>
@@ -587,7 +587,7 @@
         <v>0.35</v>
       </c>
       <c r="H5" t="n">
-        <v>460587616</v>
+        <v>450119712</v>
       </c>
     </row>
     <row r="6">
@@ -605,10 +605,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.62</v>
+        <v>1.65</v>
       </c>
       <c r="E6" t="n">
-        <v>1.63</v>
+        <v>1.61</v>
       </c>
       <c r="F6" t="n">
         <v>0.33221</v>
@@ -617,7 +617,7 @@
         <v>1.166</v>
       </c>
       <c r="H6" t="n">
-        <v>54769448</v>
+        <v>55783696</v>
       </c>
     </row>
     <row r="7">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>7.295</v>
+        <v>7.07</v>
       </c>
       <c r="E7" t="n">
-        <v>7.29</v>
+        <v>7.12</v>
       </c>
       <c r="F7" t="n">
         <v>0.97643</v>
@@ -647,7 +647,7 @@
         <v>5.387</v>
       </c>
       <c r="H7" t="n">
-        <v>10742981632</v>
+        <v>10411635712</v>
       </c>
     </row>
     <row r="8">
@@ -665,19 +665,19 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.455</v>
+        <v>1.49</v>
       </c>
       <c r="E8" t="n">
-        <v>1.44</v>
+        <v>1.5</v>
       </c>
       <c r="F8" t="n">
         <v>1.754769</v>
       </c>
       <c r="G8" t="n">
-        <v>1.125</v>
+        <v>0.984</v>
       </c>
       <c r="H8" t="n">
-        <v>3267377152</v>
+        <v>3345973760</v>
       </c>
     </row>
     <row r="9">
@@ -695,10 +695,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.58</v>
+        <v>0.61</v>
       </c>
       <c r="E9" t="n">
-        <v>0.59</v>
+        <v>0.62</v>
       </c>
       <c r="F9" t="n">
         <v>0.769921</v>
@@ -707,7 +707,7 @@
         <v>0.354</v>
       </c>
       <c r="H9" t="n">
-        <v>16707712</v>
+        <v>17571904</v>
       </c>
     </row>
     <row r="10">
@@ -725,19 +725,19 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1.13</v>
+        <v>1.17</v>
       </c>
       <c r="E10" t="n">
-        <v>1.13</v>
+        <v>1.17</v>
       </c>
       <c r="F10" t="n">
         <v>0.856341</v>
       </c>
       <c r="G10" t="n">
-        <v>1.932</v>
+        <v>1.899</v>
       </c>
       <c r="H10" t="n">
-        <v>3690704128</v>
+        <v>3852446976</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>29.6</v>
+        <v>29.52</v>
       </c>
       <c r="E11" t="n">
         <v>29.63</v>
@@ -764,10 +764,10 @@
         <v>0.916386</v>
       </c>
       <c r="G11" t="n">
-        <v>32.272</v>
+        <v>31.714</v>
       </c>
       <c r="H11" t="n">
-        <v>84227989504</v>
+        <v>85920915456</v>
       </c>
     </row>
     <row r="12">
@@ -785,10 +785,10 @@
         </is>
       </c>
       <c r="D12" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E12" t="n">
         <v>0.335</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.33</v>
       </c>
       <c r="F12" t="n">
         <v>0.615039</v>
@@ -797,7 +797,7 @@
         <v>0.448</v>
       </c>
       <c r="H12" t="n">
-        <v>121510536</v>
+        <v>119696952</v>
       </c>
     </row>
     <row r="13">
@@ -815,19 +815,19 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="E13" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="F13" t="n">
         <v>0.507856</v>
       </c>
       <c r="G13" t="n">
-        <v>0.436</v>
+        <v>0.428</v>
       </c>
       <c r="H13" t="n">
-        <v>160394240</v>
+        <v>150369600</v>
       </c>
     </row>
     <row r="14">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1.635</v>
+        <v>1.62</v>
       </c>
       <c r="E14" t="n">
         <v>1.63</v>
@@ -857,7 +857,7 @@
         <v>1.525</v>
       </c>
       <c r="H14" t="n">
-        <v>1372628224</v>
+        <v>1360035328</v>
       </c>
     </row>
     <row r="15">
@@ -875,10 +875,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2.08</v>
+        <v>2.06</v>
       </c>
       <c r="E15" t="n">
-        <v>2.06</v>
+        <v>2.05</v>
       </c>
       <c r="F15" t="n">
         <v>0.681818</v>
@@ -887,7 +887,7 @@
         <v>1.523</v>
       </c>
       <c r="H15" t="n">
-        <v>1129177856</v>
+        <v>1118320384</v>
       </c>
     </row>
     <row r="16">
@@ -905,19 +905,19 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>6.88</v>
+        <v>6.09</v>
       </c>
       <c r="E16" t="n">
-        <v>6.82</v>
+        <v>6.34</v>
       </c>
       <c r="F16" t="n">
         <v>-0.283389</v>
       </c>
       <c r="G16" t="n">
-        <v>1.598</v>
+        <v>1.458</v>
       </c>
       <c r="H16" t="n">
-        <v>5109135872</v>
+        <v>4571781120</v>
       </c>
     </row>
     <row r="17">
@@ -938,7 +938,7 @@
         <v>0.39</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4</v>
+        <v>0.395</v>
       </c>
       <c r="F17" t="n">
         <v>1.00505</v>
@@ -965,10 +965,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="E18" t="n">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="F18" t="n">
         <v>1.086437</v>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>3013980</v>
+        <v>2511649</v>
       </c>
     </row>
     <row r="19">
@@ -995,10 +995,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>6.36</v>
+        <v>6.49</v>
       </c>
       <c r="E19" t="n">
-        <v>6.35</v>
+        <v>6.5</v>
       </c>
       <c r="F19" t="n">
         <v>0.63973</v>
@@ -1007,7 +1007,7 @@
         <v>1.164</v>
       </c>
       <c r="H19" t="n">
-        <v>1415456128</v>
+        <v>1444388352</v>
       </c>
     </row>
     <row r="20">
@@ -1025,10 +1025,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2.36</v>
+        <v>2.28</v>
       </c>
       <c r="E20" t="n">
-        <v>2.36</v>
+        <v>2.35</v>
       </c>
       <c r="F20" t="n">
         <v>0.626865</v>
@@ -1037,7 +1037,7 @@
         <v>1.622</v>
       </c>
       <c r="H20" t="n">
-        <v>402443712</v>
+        <v>388801568</v>
       </c>
     </row>
     <row r="21">
@@ -1055,10 +1055,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.068</v>
+        <v>0.066</v>
       </c>
       <c r="E21" t="n">
-        <v>0.067</v>
+        <v>0.066</v>
       </c>
       <c r="F21" t="n">
         <v>0.417508</v>
@@ -1067,7 +1067,7 @@
         <v>0.005</v>
       </c>
       <c r="H21" t="n">
-        <v>75320208</v>
+        <v>73104904</v>
       </c>
     </row>
     <row r="22">
@@ -1085,10 +1085,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1.03</v>
+        <v>1.08</v>
       </c>
       <c r="E22" t="n">
-        <v>1.02</v>
+        <v>1.08</v>
       </c>
       <c r="F22" t="n">
         <v>0.7777770000000001</v>
@@ -1097,7 +1097,7 @@
         <v>0.802</v>
       </c>
       <c r="H22" t="n">
-        <v>214981600</v>
+        <v>225417616</v>
       </c>
     </row>
     <row r="23">
@@ -1115,19 +1115,19 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.61</v>
+        <v>0.66</v>
       </c>
       <c r="E23" t="n">
-        <v>0.61</v>
+        <v>0.65</v>
       </c>
       <c r="F23" t="n">
-        <v>1.190796</v>
+        <v>1.201216</v>
       </c>
       <c r="G23" t="n">
         <v>0.5570000000000001</v>
       </c>
       <c r="H23" t="n">
-        <v>41894256</v>
+        <v>45328212</v>
       </c>
     </row>
     <row r="24">
@@ -1175,19 +1175,19 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1.14</v>
+        <v>1.16</v>
       </c>
       <c r="E25" t="n">
         <v>1.14</v>
       </c>
       <c r="F25" t="n">
-        <v>0.801346</v>
+        <v>0.757877</v>
       </c>
       <c r="G25" t="n">
-        <v>0.96</v>
+        <v>0.917</v>
       </c>
       <c r="H25" t="n">
-        <v>327764800</v>
+        <v>333515072</v>
       </c>
     </row>
     <row r="26">
@@ -1205,19 +1205,19 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>8.279999999999999</v>
+        <v>8.01</v>
       </c>
       <c r="E26" t="n">
-        <v>8.199999999999999</v>
+        <v>8.08</v>
       </c>
       <c r="F26" t="n">
-        <v>0.427609</v>
+        <v>0.457711</v>
       </c>
       <c r="G26" t="n">
         <v>3.771</v>
       </c>
       <c r="H26" t="n">
-        <v>6426289664</v>
+        <v>6127602176</v>
       </c>
     </row>
     <row r="27">
@@ -1235,19 +1235,19 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.037</v>
+        <v>0.039</v>
       </c>
       <c r="E27" t="n">
-        <v>0.037</v>
+        <v>0.038</v>
       </c>
       <c r="F27" t="n">
-        <v>0.450056</v>
+        <v>0.421779</v>
       </c>
       <c r="G27" t="n">
         <v>-0.003</v>
       </c>
       <c r="H27" t="n">
-        <v>23229858</v>
+        <v>24485526</v>
       </c>
     </row>
     <row r="28">
@@ -1265,10 +1265,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9.85</v>
+        <v>10.15</v>
       </c>
       <c r="E28" t="n">
-        <v>9.85</v>
+        <v>10.15</v>
       </c>
       <c r="F28" t="n">
         <v>1.026936</v>
@@ -1277,7 +1277,7 @@
         <v>8.039999999999999</v>
       </c>
       <c r="H28" t="n">
-        <v>322041824</v>
+        <v>331850176</v>
       </c>
     </row>
     <row r="29">
@@ -1295,10 +1295,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6.8</v>
+        <v>6.94</v>
       </c>
       <c r="E29" t="n">
-        <v>6.93</v>
+        <v>6.85</v>
       </c>
       <c r="F29" t="n">
         <v>0.025813</v>
@@ -1307,7 +1307,7 @@
         <v>1.915</v>
       </c>
       <c r="H29" t="n">
-        <v>3039770112</v>
+        <v>3102353408</v>
       </c>
     </row>
     <row r="30">
@@ -1325,289 +1325,289 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.128</v>
+        <v>0.13</v>
       </c>
       <c r="E30" t="n">
-        <v>0.125</v>
+        <v>0.13</v>
       </c>
       <c r="F30" t="n">
-        <v>0.952089</v>
+        <v>0.95821</v>
       </c>
       <c r="G30" t="n">
-        <v>0.172</v>
+        <v>0.211</v>
       </c>
       <c r="H30" t="n">
-        <v>12269210</v>
+        <v>5680896</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>CVT.NZ</t>
+          <t>DGL.NZ</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Comvita Limited Ordinary Shares</t>
+          <t xml:space="preserve">Delegat Group Limited Ordinary </t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.34</v>
+        <v>14.32</v>
       </c>
       <c r="E31" t="n">
-        <v>3.3</v>
+        <v>14.1</v>
       </c>
       <c r="F31" t="n">
-        <v>1.044332</v>
+        <v>0.767676</v>
       </c>
       <c r="G31" t="n">
-        <v>3.08</v>
+        <v>4.196</v>
       </c>
       <c r="H31" t="n">
-        <v>233525792</v>
+        <v>1448181632</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>DGL.NZ</t>
+          <t>EBO.NZ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delegat Group Limited Ordinary </t>
+          <t>Ebos Group Limited Ordinary Sha</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>13.1</v>
+        <v>35.03</v>
       </c>
       <c r="E32" t="n">
-        <v>13.01</v>
+        <v>35.01</v>
       </c>
       <c r="F32" t="n">
-        <v>0.767676</v>
+        <v>0.321548</v>
       </c>
       <c r="G32" t="n">
-        <v>4.196</v>
+        <v>12.109</v>
       </c>
       <c r="H32" t="n">
-        <v>1324803072</v>
+        <v>5750839808</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>EBO.NZ</t>
+          <t>ERD.NZ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ebos Group Limited Ordinary Sha</t>
+          <t>EROAD Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>34.02</v>
+        <v>6.3</v>
       </c>
       <c r="E33" t="n">
-        <v>33.5</v>
+        <v>6.28</v>
       </c>
       <c r="F33" t="n">
-        <v>0.321548</v>
+        <v>1.167789</v>
       </c>
       <c r="G33" t="n">
-        <v>12.596</v>
+        <v>1.289</v>
       </c>
       <c r="H33" t="n">
-        <v>5585029120</v>
+        <v>515946720</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ENS.NZ</t>
+          <t>EVO.NZ</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enprise Group Limited Ordinary </t>
+          <t xml:space="preserve">Evolve Education Group Limited </t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.88</v>
+        <v>0.61</v>
       </c>
       <c r="E34" t="n">
-        <v>2.93</v>
+        <v>0.61</v>
       </c>
       <c r="F34" t="n">
-        <v>0.501683</v>
+        <v>2.646213</v>
       </c>
       <c r="G34" t="n">
-        <v>0.8</v>
+        <v>0.977</v>
       </c>
       <c r="H34" t="n">
-        <v>46534176</v>
+        <v>97324888</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ERD.NZ</t>
+          <t>FBU.NZ</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>EROAD Limited Ordinary Shares</t>
+          <t>Fletcher Building Limited Ordin</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>6.28</v>
+        <v>7.33</v>
       </c>
       <c r="E35" t="n">
-        <v>6.24</v>
+        <v>7.54</v>
       </c>
       <c r="F35" t="n">
-        <v>1.167789</v>
+        <v>1.194582</v>
       </c>
       <c r="G35" t="n">
-        <v>1.289</v>
+        <v>4.598</v>
       </c>
       <c r="H35" t="n">
-        <v>514308800</v>
+        <v>6041796608</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>EVO.NZ</t>
+          <t>FCT.NZ</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Evolve Education Group Limited </t>
+          <t>F&amp;C Investment Trust PLC Ordina</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.62</v>
+        <v>17.5</v>
       </c>
       <c r="E36" t="n">
-        <v>0.64</v>
+        <v>17.95</v>
       </c>
       <c r="F36" t="n">
-        <v>2.722222</v>
+        <v>0.800224</v>
       </c>
       <c r="G36" t="n">
-        <v>0.783</v>
+        <v>13.416</v>
       </c>
       <c r="H36" t="n">
-        <v>98920376</v>
+        <v>9527069696</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>FBU.NZ</t>
+          <t>FPH.NZ</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Fletcher Building Limited Ordin</t>
+          <t>Fisher &amp; Paykel Healthcare Corp</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.68</v>
+        <v>32.25</v>
       </c>
       <c r="E37" t="n">
-        <v>7.72</v>
+        <v>31.98</v>
       </c>
       <c r="F37" t="n">
-        <v>1.168911</v>
+        <v>-0.156992</v>
       </c>
       <c r="G37" t="n">
-        <v>4.598</v>
+        <v>2.639</v>
       </c>
       <c r="H37" t="n">
-        <v>6306447360</v>
+        <v>18587224064</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FCT.NZ</t>
+          <t>FRE.NZ</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>F&amp;C Investment Trust PLC Ordina</t>
+          <t>Freightways Limited Ordinary Sh</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>17.9</v>
+        <v>12.55</v>
       </c>
       <c r="E38" t="n">
-        <v>17.9</v>
+        <v>12.69</v>
       </c>
       <c r="F38" t="n">
-        <v>0.800224</v>
+        <v>0.948933</v>
       </c>
       <c r="G38" t="n">
-        <v>13.641</v>
+        <v>2.06</v>
       </c>
       <c r="H38" t="n">
-        <v>9744830464</v>
+        <v>2077501952</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>FPH.NZ</t>
+          <t>FSF.NZ</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Fisher &amp; Paykel Healthcare Corp</t>
+          <t>Fonterra Shareholders' Fund Uni</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>33.59</v>
+        <v>3.7</v>
       </c>
       <c r="E39" t="n">
-        <v>33.5</v>
+        <v>3.7</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.207631</v>
+        <v>0.083471</v>
       </c>
       <c r="G39" t="n">
-        <v>2.639</v>
+        <v>4.542</v>
       </c>
       <c r="H39" t="n">
-        <v>19359561728</v>
+        <v>394841792</v>
       </c>
     </row>
     <row r="40">
@@ -1616,58 +1616,58 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>FSF.NZ</t>
+          <t>FWL.NZ</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Fonterra Shareholders' Fund Uni</t>
+          <t>Foley Wines Limited Ordinary Sh</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>3.74</v>
+        <v>1.49</v>
       </c>
       <c r="E40" t="n">
-        <v>3.7</v>
+        <v>1.47</v>
       </c>
       <c r="F40" t="n">
-        <v>0.06386500000000001</v>
+        <v>0.410724</v>
       </c>
       <c r="G40" t="n">
-        <v>4.542</v>
+        <v>2.013</v>
       </c>
       <c r="H40" t="n">
-        <v>399110368</v>
+        <v>97946792</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>FWL.NZ</t>
+          <t>GEN.NZ</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Foley Wines Limited Ordinary Sh</t>
+          <t>General Capital Limited Ordinar</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.49</v>
+        <v>0.056</v>
       </c>
       <c r="E41" t="n">
-        <v>1.5</v>
+        <v>0.056</v>
       </c>
       <c r="F41" t="n">
-        <v>0.44725</v>
+        <v>-0.092281</v>
       </c>
       <c r="G41" t="n">
-        <v>1.918</v>
+        <v>0.061</v>
       </c>
       <c r="H41" t="n">
-        <v>97946792</v>
+        <v>9052848</v>
       </c>
     </row>
     <row r="42">
@@ -1676,28 +1676,28 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>GEN.NZ</t>
+          <t>GEO.NZ</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>General Capital Limited Ordinar</t>
+          <t>Geo Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.055</v>
+        <v>0.115</v>
       </c>
       <c r="E42" t="n">
-        <v>0.057</v>
+        <v>0.118</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.10882</v>
+        <v>1.57435</v>
       </c>
       <c r="G42" t="n">
-        <v>0.061</v>
+        <v>0.007</v>
       </c>
       <c r="H42" t="n">
-        <v>8958070</v>
+        <v>13072740</v>
       </c>
     </row>
     <row r="43">
@@ -1706,28 +1706,28 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GEO.NZ</t>
+          <t>GFL.NZ</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Geo Limited Ordinary Shares</t>
+          <t>Geneva Finance Limited Ordinary</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.118</v>
+        <v>0.73</v>
       </c>
       <c r="E43" t="n">
-        <v>0.12</v>
+        <v>0.72</v>
       </c>
       <c r="F43" t="n">
-        <v>1.53872</v>
+        <v>0.181868</v>
       </c>
       <c r="G43" t="n">
-        <v>0.016</v>
+        <v>0.448</v>
       </c>
       <c r="H43" t="n">
-        <v>13413768</v>
+        <v>53242768</v>
       </c>
     </row>
     <row r="44">
@@ -1736,28 +1736,28 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GFL.NZ</t>
+          <t>GMT.NZ</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Geneva Finance Limited Ordinary</t>
+          <t>Goodman Property Trust (NS) Ord</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.76</v>
+        <v>2.65</v>
       </c>
       <c r="E44" t="n">
-        <v>0.76</v>
+        <v>2.62</v>
       </c>
       <c r="F44" t="n">
-        <v>0.122895</v>
+        <v>0.097844</v>
       </c>
       <c r="G44" t="n">
-        <v>0.447</v>
+        <v>2.134</v>
       </c>
       <c r="H44" t="n">
-        <v>55430824</v>
+        <v>3702844928</v>
       </c>
     </row>
     <row r="45">
@@ -1766,28 +1766,28 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>GMT.NZ</t>
+          <t>GNE.NZ</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Goodman Property Trust (NS) Ord</t>
+          <t>Genesis Energy Limited Ordinary</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2.62</v>
+        <v>3.38</v>
       </c>
       <c r="E45" t="n">
-        <v>2.6</v>
+        <v>3.38</v>
       </c>
       <c r="F45" t="n">
-        <v>0.071829</v>
+        <v>0.5394949999999999</v>
       </c>
       <c r="G45" t="n">
-        <v>2.134</v>
+        <v>1.816</v>
       </c>
       <c r="H45" t="n">
-        <v>3660925696</v>
+        <v>3527266560</v>
       </c>
     </row>
     <row r="46">
@@ -1796,28 +1796,28 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>GNE.NZ</t>
+          <t>GSH.NZ</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Genesis Energy Limited Ordinary</t>
+          <t>Good Spirits Hospitality Limite</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>3.37</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E46" t="n">
-        <v>3.335</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="F46" t="n">
-        <v>0.537598</v>
+        <v>-0.129353</v>
       </c>
       <c r="G46" t="n">
-        <v>1.816</v>
+        <v>0.127</v>
       </c>
       <c r="H46" t="n">
-        <v>3516830720</v>
+        <v>4041415</v>
       </c>
     </row>
     <row r="47">
@@ -1826,28 +1826,28 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>GSH.NZ</t>
+          <t>GTK.NZ</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Good Spirits Hospitality Limite</t>
+          <t>Gentrack Group Limited Ordinary</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.07000000000000001</v>
+        <v>2</v>
       </c>
       <c r="E47" t="n">
-        <v>0.07000000000000001</v>
+        <v>2.02</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.14927</v>
+        <v>1.381426</v>
       </c>
       <c r="G47" t="n">
-        <v>0.127</v>
+        <v>1.65</v>
       </c>
       <c r="H47" t="n">
-        <v>4041415</v>
+        <v>197789600</v>
       </c>
     </row>
     <row r="48">
@@ -1856,28 +1856,28 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>GTK.NZ</t>
+          <t>GWC.NZ</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Gentrack Group Limited Ordinary</t>
+          <t>Goodwood Capital Limited Ordina</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1.98</v>
+        <v>0.027</v>
       </c>
       <c r="E48" t="n">
-        <v>1.97</v>
+        <v>0.027</v>
       </c>
       <c r="F48" t="n">
-        <v>1.393939</v>
+        <v>-0.470978</v>
       </c>
       <c r="G48" t="n">
-        <v>1.65</v>
+        <v>-0.018</v>
       </c>
       <c r="H48" t="n">
-        <v>195811712</v>
+        <v>882624</v>
       </c>
     </row>
     <row r="49">
@@ -1886,28 +1886,28 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>GWC.NZ</t>
+          <t>GXH.NZ</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Goodwood Capital Limited Ordina</t>
+          <t>Green Cross Health Limited Ordi</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.027</v>
+        <v>1.15</v>
       </c>
       <c r="E49" t="n">
-        <v>0.027</v>
+        <v>1.13</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.433782</v>
+        <v>0.380873</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.004</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="H49" t="n">
-        <v>882624</v>
+        <v>164625936</v>
       </c>
     </row>
     <row r="50">
@@ -1916,28 +1916,28 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>GXH.NZ</t>
+          <t>HFL.NZ</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Green Cross Health Limited Ordi</t>
+          <t>Henderson Far East Income Limit</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1.12</v>
+        <v>6.24</v>
       </c>
       <c r="E50" t="n">
-        <v>1.11</v>
+        <v>6.24</v>
       </c>
       <c r="F50" t="n">
-        <v>0.333894</v>
+        <v>0.67789</v>
       </c>
       <c r="G50" t="n">
-        <v>0.986</v>
+        <v>4.486</v>
       </c>
       <c r="H50" t="n">
-        <v>160331344</v>
+        <v>887945792</v>
       </c>
     </row>
     <row r="51">
@@ -1946,28 +1946,28 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>HFL.NZ</t>
+          <t>HGH.NZ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Henderson Far East Income Limit</t>
+          <t>Heartland Group Holdings Limite</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>6.2</v>
+        <v>2.26</v>
       </c>
       <c r="E51" t="n">
-        <v>6.24</v>
+        <v>2.24</v>
       </c>
       <c r="F51" t="n">
-        <v>0.67789</v>
+        <v>1.144831</v>
       </c>
       <c r="G51" t="n">
-        <v>4.565</v>
+        <v>1.263</v>
       </c>
       <c r="H51" t="n">
-        <v>882253824</v>
+        <v>1318531456</v>
       </c>
     </row>
     <row r="52">
@@ -1976,58 +1976,58 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>HGH.NZ</t>
+          <t>HLG.NZ</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Heartland Group Holdings Limite</t>
+          <t>Hallenstein Glasson Holdings Li</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2.17</v>
+        <v>7.05</v>
       </c>
       <c r="E52" t="n">
-        <v>2.1</v>
+        <v>7.12</v>
       </c>
       <c r="F52" t="n">
-        <v>1.093714</v>
+        <v>1.205898</v>
       </c>
       <c r="G52" t="n">
-        <v>1.263</v>
+        <v>1.389</v>
       </c>
       <c r="H52" t="n">
-        <v>1266023552</v>
+        <v>420526176</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>HLG.NZ</t>
+          <t>IFT.NZ</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Hallenstein Glasson Holdings Li</t>
+          <t>Infratil Limited Ordinary Share</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6.76</v>
+        <v>7.39</v>
       </c>
       <c r="E53" t="n">
-        <v>6.72</v>
+        <v>7.35</v>
       </c>
       <c r="F53" t="n">
-        <v>1.230078</v>
+        <v>0.896075</v>
       </c>
       <c r="G53" t="n">
-        <v>1.389</v>
+        <v>3.657</v>
       </c>
       <c r="H53" t="n">
-        <v>403227936</v>
+        <v>5342622720</v>
       </c>
     </row>
     <row r="54">
@@ -2036,28 +2036,28 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>IFT.NZ</t>
+          <t>IKE.NZ</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Infratil Limited Ordinary Share</t>
+          <t>ikeGPS Group Limited Ordinary S</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>7.475</v>
+        <v>1.05</v>
       </c>
       <c r="E54" t="n">
-        <v>7.48</v>
+        <v>1.05</v>
       </c>
       <c r="F54" t="n">
-        <v>0.880471</v>
+        <v>0.554433</v>
       </c>
       <c r="G54" t="n">
-        <v>3.657</v>
+        <v>0.161</v>
       </c>
       <c r="H54" t="n">
-        <v>5404073984</v>
+        <v>140156096</v>
       </c>
     </row>
     <row r="55">
@@ -2066,28 +2066,28 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>IKE.NZ</t>
+          <t>IPL.NZ</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ikeGPS Group Limited Ordinary S</t>
+          <t>Investore Property Limited (NS)</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>1.08</v>
+        <v>2.02</v>
       </c>
       <c r="E55" t="n">
-        <v>1.04</v>
+        <v>2.04</v>
       </c>
       <c r="F55" t="n">
-        <v>0.554433</v>
+        <v>0.184181</v>
       </c>
       <c r="G55" t="n">
-        <v>0.163</v>
+        <v>2.08</v>
       </c>
       <c r="H55" t="n">
-        <v>144160560</v>
+        <v>743632704</v>
       </c>
     </row>
     <row r="56">
@@ -2096,28 +2096,28 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>IPL.NZ</t>
+          <t>JLG.NZ</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Investore Property Limited (NS)</t>
+          <t>Just Life Group Limited Ordinar</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>2.01</v>
+        <v>0.91</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>0.92</v>
       </c>
       <c r="F56" t="n">
-        <v>0.184624</v>
+        <v>0.563025</v>
       </c>
       <c r="G56" t="n">
-        <v>2.08</v>
+        <v>0.208</v>
       </c>
       <c r="H56" t="n">
-        <v>739951360</v>
+        <v>84443816</v>
       </c>
     </row>
     <row r="57">
@@ -2126,28 +2126,28 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>JLG.NZ</t>
+          <t>JPG.NZ</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Just Life Group Limited Ordinar</t>
+          <t>JPMorgan Global Growth &amp; Income</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.87</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="E57" t="n">
-        <v>0.87</v>
+        <v>9.26</v>
       </c>
       <c r="F57" t="n">
-        <v>0.607182</v>
+        <v>0.6661049999999999</v>
       </c>
       <c r="G57" t="n">
-        <v>0.208</v>
+        <v>5.469</v>
       </c>
       <c r="H57" t="n">
-        <v>80732000</v>
+        <v>1248397184</v>
       </c>
     </row>
     <row r="58">
@@ -2156,88 +2156,88 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>JPG.NZ</t>
+          <t>KFL.NZ</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>JPMorgan Global Growth &amp; Income</t>
+          <t>Kingfish Limited Ordinary Share</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>8.949999999999999</v>
+        <v>2.04</v>
       </c>
       <c r="E58" t="n">
-        <v>8.949999999999999</v>
+        <v>2.04</v>
       </c>
       <c r="F58" t="n">
-        <v>0.6661049999999999</v>
+        <v>0.630735</v>
       </c>
       <c r="G58" t="n">
-        <v>5.619</v>
+        <v>1.675</v>
       </c>
       <c r="H58" t="n">
-        <v>1211838848</v>
+        <v>507119520</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>KFL.NZ</t>
+          <t>KMD.NZ</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Kingfish Limited Ordinary Share</t>
+          <t>Kathmandu Holdings Limited Ordi</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>2.02</v>
+        <v>1.34</v>
       </c>
       <c r="E59" t="n">
-        <v>2.01</v>
+        <v>1.36</v>
       </c>
       <c r="F59" t="n">
-        <v>0.632996</v>
+        <v>1.243228</v>
       </c>
       <c r="G59" t="n">
-        <v>1.767</v>
+        <v>1.096</v>
       </c>
       <c r="H59" t="n">
-        <v>630314688</v>
+        <v>950061376</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>KMD.NZ</t>
+          <t>KPG.NZ</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Kathmandu Holdings Limited Ordi</t>
+          <t>Kiwi Property Group Limited Ord</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>1.29</v>
+        <v>1.165</v>
       </c>
       <c r="E60" t="n">
-        <v>1.28</v>
+        <v>1.155</v>
       </c>
       <c r="F60" t="n">
-        <v>1.200336</v>
+        <v>0.514096</v>
       </c>
       <c r="G60" t="n">
-        <v>1.096</v>
+        <v>1.36</v>
       </c>
       <c r="H60" t="n">
-        <v>914611264</v>
+        <v>1829154816</v>
       </c>
     </row>
     <row r="61">
@@ -2246,28 +2246,28 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>KPG.NZ</t>
+          <t>MCK.NZ</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Kiwi Property Group Limited Ord</t>
+          <t>Millennium &amp; Copthorne Hotels N</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>1.145</v>
+        <v>2.41</v>
       </c>
       <c r="E61" t="n">
-        <v>1.14</v>
+        <v>2.44</v>
       </c>
       <c r="F61" t="n">
-        <v>0.51964</v>
+        <v>0.833056</v>
       </c>
       <c r="G61" t="n">
-        <v>1.36</v>
+        <v>4.7</v>
       </c>
       <c r="H61" t="n">
-        <v>1797752960</v>
+        <v>254204400</v>
       </c>
     </row>
     <row r="62">
@@ -2276,868 +2276,868 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>LIC.NZ</t>
+          <t>MCY.NZ</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Livestock Improvement Corporati</t>
+          <t>Mercury NZ Limited Ordinary Sha</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>1.2</v>
+        <v>6.8</v>
       </c>
       <c r="E62" t="n">
-        <v>1.2</v>
+        <v>6.8</v>
       </c>
       <c r="F62" t="n">
-        <v>0.10101</v>
+        <v>0.537815</v>
       </c>
       <c r="G62" t="n">
-        <v>2.066</v>
+        <v>2.709</v>
       </c>
       <c r="H62" t="n">
-        <v>152498400</v>
+        <v>9263640576</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>MCK.NZ</t>
+          <t>MEL.NZ</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Millennium &amp; Copthorne Hotels N</t>
+          <t>Meridian Energy Limited (NS) Or</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>2.45</v>
+        <v>5.07</v>
       </c>
       <c r="E63" t="n">
-        <v>2.45</v>
+        <v>5.02</v>
       </c>
       <c r="F63" t="n">
-        <v>0.914141</v>
+        <v>0.714927</v>
       </c>
       <c r="G63" t="n">
-        <v>4.7</v>
+        <v>1.958</v>
       </c>
       <c r="H63" t="n">
-        <v>258423552</v>
+        <v>12992331776</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>MCY.NZ</t>
+          <t>MFT.NZ</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Mercury NZ Limited Ordinary Sha</t>
+          <t>Mainfreight Limited Ordinary Sh</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>6.91</v>
+        <v>92.41</v>
       </c>
       <c r="E64" t="n">
-        <v>6.82</v>
+        <v>91.91</v>
       </c>
       <c r="F64" t="n">
-        <v>0.537037</v>
+        <v>0.531007</v>
       </c>
       <c r="G64" t="n">
-        <v>3.073</v>
+        <v>9.885999999999999</v>
       </c>
       <c r="H64" t="n">
-        <v>9413492736</v>
+        <v>9305594880</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>MEL.NZ</t>
+          <t>MHJ.NZ</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Meridian Energy Limited (NS) Or</t>
+          <t xml:space="preserve">Michael Hill International Ltd </t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>5.255</v>
+        <v>0.88</v>
       </c>
       <c r="E65" t="n">
-        <v>5.28</v>
+        <v>0.88</v>
       </c>
       <c r="F65" t="n">
-        <v>0.714927</v>
+        <v>1.634955</v>
       </c>
       <c r="G65" t="n">
-        <v>1.958</v>
+        <v>0.704</v>
       </c>
       <c r="H65" t="n">
-        <v>13466409984</v>
+        <v>343487776</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>MFT.NZ</t>
+          <t>MHM.NZ</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Mainfreight Limited Ordinary Sh</t>
+          <t>MHM Automation Limited</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>90.5</v>
+        <v>0.67</v>
       </c>
       <c r="E66" t="n">
-        <v>90.01000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="F66" t="n">
-        <v>0.52918</v>
+        <v>2.036484</v>
       </c>
       <c r="G66" t="n">
-        <v>11.073</v>
+        <v>0.074</v>
       </c>
       <c r="H66" t="n">
-        <v>9113259008</v>
+        <v>43964800</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>MHJ.NZ</t>
+          <t>MLN.NZ</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Michael Hill International Ltd </t>
+          <t xml:space="preserve">Marlin Global Limited Ordinary </t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.89</v>
+        <v>1.5</v>
       </c>
       <c r="E67" t="n">
-        <v>0.88</v>
+        <v>1.53</v>
       </c>
       <c r="F67" t="n">
-        <v>1.626823</v>
+        <v>0.699281</v>
       </c>
       <c r="G67" t="n">
-        <v>0.72</v>
+        <v>1.099</v>
       </c>
       <c r="H67" t="n">
-        <v>345303072</v>
+        <v>227847008</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>MHM.NZ</t>
+          <t>MMH.NZ</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>MHM Automation Limited</t>
+          <t>Marsden Maritime Holdings Limit</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.64</v>
+        <v>6.3</v>
       </c>
       <c r="E68" t="n">
-        <v>0.63</v>
+        <v>6.13</v>
       </c>
       <c r="F68" t="n">
-        <v>1.935465</v>
+        <v>0.381426</v>
       </c>
       <c r="G68" t="n">
-        <v>0.074</v>
+        <v>3.361</v>
       </c>
       <c r="H68" t="n">
-        <v>41996224</v>
+        <v>260194416</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>MLN.NZ</t>
+          <t>MPG.NZ</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Marlin Global Limited Ordinary </t>
+          <t>Metro Performance Glass Limited</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>1.5</v>
+        <v>0.44</v>
       </c>
       <c r="E69" t="n">
-        <v>1.48</v>
+        <v>0.445</v>
       </c>
       <c r="F69" t="n">
-        <v>0.6969689999999999</v>
+        <v>0.273079</v>
       </c>
       <c r="G69" t="n">
-        <v>1.099</v>
+        <v>0.453</v>
       </c>
       <c r="H69" t="n">
-        <v>227847008</v>
+        <v>81566320</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>MMH.NZ</t>
+          <t>MWE.NZ</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Marsden Maritime Holdings Limit</t>
+          <t xml:space="preserve">Marlborough Wine Estates Group </t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>6.2</v>
+        <v>0.255</v>
       </c>
       <c r="E70" t="n">
-        <v>6.2</v>
+        <v>0.245</v>
       </c>
       <c r="F70" t="n">
-        <v>0.365319</v>
+        <v>0.052486</v>
       </c>
       <c r="G70" t="n">
-        <v>3.361</v>
+        <v>0.058</v>
       </c>
       <c r="H70" t="n">
-        <v>256064336</v>
+        <v>75723264</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>MPG.NZ</t>
+          <t>NTL.NZ</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Metro Performance Glass Limited</t>
+          <t>New Talisman Gold Mines Limited</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.44</v>
+        <v>0.003</v>
       </c>
       <c r="E71" t="n">
-        <v>0.44</v>
+        <v>0.003</v>
       </c>
       <c r="F71" t="n">
-        <v>0.273288</v>
+        <v>-0.355444</v>
       </c>
       <c r="G71" t="n">
-        <v>0.453</v>
+        <v>0.006</v>
       </c>
       <c r="H71" t="n">
-        <v>81566320</v>
+        <v>8376689</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>MWE.NZ</t>
+          <t>NWF.NZ</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Marlborough Wine Estates Group </t>
+          <t>NZ Windfarms Limited Ordinary S</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.245</v>
+        <v>0.275</v>
       </c>
       <c r="E72" t="n">
-        <v>0.245</v>
+        <v>0.28</v>
       </c>
       <c r="F72" t="n">
-        <v>-0.040965</v>
+        <v>0.099159</v>
       </c>
       <c r="G72" t="n">
-        <v>0.058</v>
+        <v>0.132</v>
       </c>
       <c r="H72" t="n">
-        <v>72753728</v>
+        <v>79217600</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>NPH.NZ</t>
+          <t>NZK.NZ</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Napier Port Holdings Limited Or</t>
+          <t>NZ King Salmon Investments Limi</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>3.23</v>
+        <v>1.44</v>
       </c>
       <c r="E73" t="n">
-        <v>3.19</v>
+        <v>1.45</v>
       </c>
       <c r="F73" t="n">
-        <v>0.79852</v>
+        <v>0.352723</v>
       </c>
       <c r="G73" t="n">
-        <v>1.639</v>
+        <v>1.388</v>
       </c>
       <c r="H73" t="n">
-        <v>645599488</v>
+        <v>200139840</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>NTL.NZ</t>
+          <t>NZM.NZ</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>New Talisman Gold Mines Limited</t>
+          <t>NZME Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.003</v>
+        <v>0.95</v>
       </c>
       <c r="E74" t="n">
-        <v>0.003</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F74" t="n">
-        <v>-0.081369</v>
+        <v>1.351381</v>
       </c>
       <c r="G74" t="n">
-        <v>0.006</v>
+        <v>0.668</v>
       </c>
       <c r="H74" t="n">
-        <v>8376689</v>
+        <v>187691504</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>NWF.NZ</t>
+          <t>NZO.NZ</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>NZ Windfarms Limited Ordinary S</t>
+          <t>New Zealand Oil &amp; Gas Ltd Ordin</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.27</v>
+        <v>0.415</v>
       </c>
       <c r="E75" t="n">
-        <v>0.27</v>
+        <v>0.415</v>
       </c>
       <c r="F75" t="n">
-        <v>0.171717</v>
+        <v>0.445938</v>
       </c>
       <c r="G75" t="n">
-        <v>0.132</v>
+        <v>0.614</v>
       </c>
       <c r="H75" t="n">
-        <v>77777280</v>
+        <v>68238864</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>NZK.NZ</t>
+          <t>NZR.NZ</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>NZ King Salmon Investments Limi</t>
+          <t>The New Zealand Refining Compan</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>1.43</v>
+        <v>0.9</v>
       </c>
       <c r="E76" t="n">
-        <v>1.41</v>
+        <v>0.9</v>
       </c>
       <c r="F76" t="n">
-        <v>0.372474</v>
+        <v>1.017136</v>
       </c>
       <c r="G76" t="n">
-        <v>1.388</v>
+        <v>1.805</v>
       </c>
       <c r="H76" t="n">
-        <v>198749968</v>
+        <v>282136480</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>NZM.NZ</t>
+          <t>NZX.NZ</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>NZME Limited Ordinary Shares</t>
+          <t>NZX Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.93</v>
+        <v>1.82</v>
       </c>
       <c r="E77" t="n">
-        <v>0.93</v>
+        <v>1.86</v>
       </c>
       <c r="F77" t="n">
-        <v>1.341189</v>
+        <v>0.630735</v>
       </c>
       <c r="G77" t="n">
-        <v>0.668</v>
+        <v>0.243</v>
       </c>
       <c r="H77" t="n">
-        <v>183740096</v>
+        <v>505961824</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>NZO.NZ</t>
+          <t>OCA.NZ</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>New Zealand Oil &amp; Gas Ltd Ordin</t>
+          <t>Oceania Healthcare Limited Ordi</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.405</v>
+        <v>1.51</v>
       </c>
       <c r="E78" t="n">
-        <v>0.4</v>
+        <v>1.5</v>
       </c>
       <c r="F78" t="n">
-        <v>0.468574</v>
+        <v>0.765714</v>
       </c>
       <c r="G78" t="n">
-        <v>0.614</v>
+        <v>1.217</v>
       </c>
       <c r="H78" t="n">
-        <v>66594560</v>
+        <v>1059630464</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>NZR.NZ</t>
+          <t>PCT.NZ</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>The New Zealand Refining Compan</t>
+          <t>Precinct Properties New Zealand</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.9</v>
+        <v>1.695</v>
       </c>
       <c r="E79" t="n">
-        <v>0.87</v>
+        <v>1.7</v>
       </c>
       <c r="F79" t="n">
-        <v>1.021885</v>
+        <v>0.081813</v>
       </c>
       <c r="G79" t="n">
-        <v>1.848</v>
+        <v>1.549</v>
       </c>
       <c r="H79" t="n">
-        <v>282136480</v>
+        <v>2226823168</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>NZX.NZ</t>
+          <t>PEB.NZ</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>NZX Limited Ordinary Shares</t>
+          <t>Pacific Edge Limited Ordinary S</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>1.87</v>
+        <v>1.34</v>
       </c>
       <c r="E80" t="n">
-        <v>1.85</v>
+        <v>1.39</v>
       </c>
       <c r="F80" t="n">
-        <v>0.650953</v>
+        <v>0.5669459999999999</v>
       </c>
       <c r="G80" t="n">
-        <v>0.243</v>
+        <v>0.035</v>
       </c>
       <c r="H80" t="n">
-        <v>519861856</v>
+        <v>975223872</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>OCA.NZ</t>
+          <t>PFI.NZ</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Oceania Healthcare Limited Ordi</t>
+          <t>Property For Industry Limited O</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>1.48</v>
+        <v>3</v>
       </c>
       <c r="E81" t="n">
-        <v>1.46</v>
+        <v>3.03</v>
       </c>
       <c r="F81" t="n">
-        <v>0.754325</v>
+        <v>0.377003</v>
       </c>
       <c r="G81" t="n">
-        <v>1.217</v>
+        <v>2.267</v>
       </c>
       <c r="H81" t="n">
-        <v>1038578176</v>
+        <v>1507479040</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>PCT.NZ</t>
+          <t>PGW.NZ</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Precinct Properties New Zealand</t>
+          <t xml:space="preserve">PGG Wrightson Limited Ordinary </t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>1.67</v>
+        <v>3.68</v>
       </c>
       <c r="E82" t="n">
-        <v>1.67</v>
+        <v>3.72</v>
       </c>
       <c r="F82" t="n">
-        <v>0.061728</v>
+        <v>0.95681</v>
       </c>
       <c r="G82" t="n">
-        <v>1.523</v>
+        <v>2.357</v>
       </c>
       <c r="H82" t="n">
-        <v>2468660736</v>
+        <v>277781472</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>PEB.NZ</t>
+          <t>PHL.NZ</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Pacific Edge Limited Ordinary S</t>
+          <t>Promisia Healthcare Limited Ord</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>1.35</v>
+        <v>0.001</v>
       </c>
       <c r="E83" t="n">
-        <v>1.35</v>
+        <v>0.001</v>
       </c>
       <c r="F83" t="n">
-        <v>0.587542</v>
+        <v>0.496406</v>
       </c>
       <c r="G83" t="n">
-        <v>0.035</v>
+        <v>-0.001</v>
       </c>
       <c r="H83" t="n">
-        <v>984105408</v>
+        <v>21274700</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>PFI.NZ</t>
+          <t>POT.NZ</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Property For Industry Limited O</t>
+          <t>Port of Tauranga Ltd Ordinary S</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2.99</v>
+        <v>7.38</v>
       </c>
       <c r="E84" t="n">
-        <v>2.97</v>
+        <v>7.15</v>
       </c>
       <c r="F84" t="n">
-        <v>0.356341</v>
+        <v>0.533996</v>
       </c>
       <c r="G84" t="n">
-        <v>2.772</v>
+        <v>1.759</v>
       </c>
       <c r="H84" t="n">
-        <v>1505402240</v>
+        <v>5020370432</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>PGW.NZ</t>
+          <t>PPH.NZ</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">PGG Wrightson Limited Ordinary </t>
+          <t>Pushpay Holdings Limited Ordina</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>3.5</v>
+        <v>1.76</v>
       </c>
       <c r="E85" t="n">
-        <v>3.43</v>
+        <v>1.75</v>
       </c>
       <c r="F85" t="n">
-        <v>0.964646</v>
+        <v>0.980652</v>
       </c>
       <c r="G85" t="n">
-        <v>2.299</v>
+        <v>0.122</v>
       </c>
       <c r="H85" t="n">
-        <v>264194336</v>
+        <v>1951540736</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>PHL.NZ</t>
+          <t>PX1.NZ</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Promisia Healthcare Limited Ord</t>
+          <t xml:space="preserve">Plexure Group Limited Ordinary </t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.001</v>
+        <v>0.54</v>
       </c>
       <c r="E86" t="n">
-        <v>0.001</v>
+        <v>0.57</v>
       </c>
       <c r="F86" t="n">
-        <v>0.5157119999999999</v>
+        <v>0.10503</v>
       </c>
       <c r="G86" t="n">
-        <v>0.001</v>
+        <v>0.245</v>
       </c>
       <c r="H86" t="n">
-        <v>21285000</v>
+        <v>93658680</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>POT.NZ</t>
+          <t>PYS.NZ</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Port of Tauranga Ltd Ordinary S</t>
+          <t>PaySauce Limited Ordinary Share</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>7.2</v>
+        <v>0.32</v>
       </c>
       <c r="E87" t="n">
-        <v>7.22</v>
+        <v>0.325</v>
       </c>
       <c r="F87" t="n">
-        <v>0.56734</v>
+        <v>1.095342</v>
       </c>
       <c r="G87" t="n">
-        <v>1.759</v>
+        <v>0.018</v>
       </c>
       <c r="H87" t="n">
-        <v>4897922560</v>
+        <v>44301440</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>PPH.NZ</t>
+          <t>QEX.NZ</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Pushpay Holdings Limited Ordina</t>
+          <t xml:space="preserve">QEX Logistics Limited Ordinary </t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>1.74</v>
+        <v>0.285</v>
       </c>
       <c r="E88" t="n">
-        <v>1.68</v>
+        <v>0.285</v>
       </c>
       <c r="F88" t="n">
-        <v>0.888888</v>
+        <v>1.144887</v>
       </c>
       <c r="G88" t="n">
-        <v>0.125</v>
+        <v>0.143</v>
       </c>
       <c r="H88" t="n">
-        <v>1929068416</v>
+        <v>16142571</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>PX1.NZ</t>
+          <t>RAK.NZ</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Plexure Group Limited Ordinary </t>
+          <t>Rakon Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="E89" t="n">
-        <v>0.57</v>
+        <v>0.97</v>
       </c>
       <c r="F89" t="n">
-        <v>0.080808</v>
+        <v>1.286898</v>
       </c>
       <c r="G89" t="n">
-        <v>0.245</v>
+        <v>0.458</v>
       </c>
       <c r="H89" t="n">
-        <v>97127520</v>
+        <v>217602256</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>PYS.NZ</t>
+          <t>RBD.NZ</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>PaySauce Limited Ordinary Share</t>
+          <t>Restaurant Brands NZ Limited Or</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.33</v>
+        <v>16</v>
       </c>
       <c r="E90" t="n">
-        <v>0.32</v>
+        <v>15.61</v>
       </c>
       <c r="F90" t="n">
-        <v>1.052509</v>
+        <v>0.915422</v>
       </c>
       <c r="G90" t="n">
-        <v>0.018</v>
+        <v>1.847</v>
       </c>
       <c r="H90" t="n">
-        <v>45685860</v>
+        <v>1996144000</v>
       </c>
     </row>
     <row r="91">
@@ -3146,1108 +3146,1048 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>QEX.NZ</t>
+          <t>RYM.NZ</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve">QEX Logistics Limited Ordinary </t>
+          <t>Ryman Healthcare Limited Ordina</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0.285</v>
+        <v>15.3</v>
       </c>
       <c r="E91" t="n">
-        <v>0.285</v>
+        <v>15.13</v>
       </c>
       <c r="F91" t="n">
-        <v>1.129198</v>
+        <v>0.820342</v>
       </c>
       <c r="G91" t="n">
-        <v>0.143</v>
+        <v>5.689</v>
       </c>
       <c r="H91" t="n">
-        <v>16142599</v>
+        <v>7649999872</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>RAK.NZ</t>
+          <t>SAN.NZ</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Rakon Limited Ordinary Shares</t>
+          <t>Sanford Limited (NS) Ordinary S</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0.95</v>
+        <v>4.6</v>
       </c>
       <c r="E92" t="n">
-        <v>0.95</v>
+        <v>4.64</v>
       </c>
       <c r="F92" t="n">
-        <v>1.310886</v>
+        <v>0.248203</v>
       </c>
       <c r="G92" t="n">
-        <v>0.458</v>
+        <v>6.848</v>
       </c>
       <c r="H92" t="n">
-        <v>217602256</v>
+        <v>430128032</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>RBD.NZ</t>
+          <t>SCL.NZ</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Restaurant Brands NZ Limited Or</t>
+          <t>Scales Corporation Limited Ordi</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>15.7</v>
+        <v>5.1</v>
       </c>
       <c r="E93" t="n">
-        <v>15.5</v>
+        <v>4.95</v>
       </c>
       <c r="F93" t="n">
-        <v>0.929854</v>
+        <v>0.191265</v>
       </c>
       <c r="G93" t="n">
-        <v>1.847</v>
+        <v>2.63</v>
       </c>
       <c r="H93" t="n">
-        <v>1958716288</v>
+        <v>724664128</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>RYM.NZ</t>
+          <t>SCT.NZ</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Ryman Healthcare Limited Ordina</t>
+          <t>Scott Technology Limited Ordina</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>14.95</v>
+        <v>2.91</v>
       </c>
       <c r="E94" t="n">
-        <v>14.93</v>
+        <v>2.82</v>
       </c>
       <c r="F94" t="n">
-        <v>0.827721</v>
+        <v>0.669983</v>
       </c>
       <c r="G94" t="n">
-        <v>5.689</v>
+        <v>1.198</v>
       </c>
       <c r="H94" t="n">
-        <v>7474999808</v>
+        <v>227885024</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>SAN.NZ</t>
+          <t>SCY.NZ</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Sanford Limited (NS) Ordinary S</t>
+          <t>Smiths City Group Limited Ordin</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>4.7</v>
+        <v>0.14</v>
       </c>
       <c r="E95" t="n">
-        <v>4.7</v>
+        <v>0.14</v>
       </c>
       <c r="F95" t="n">
-        <v>0.232884</v>
+        <v>1.146218</v>
       </c>
       <c r="G95" t="n">
-        <v>6.848</v>
+        <v>0.697</v>
       </c>
       <c r="H95" t="n">
-        <v>439478624</v>
+        <v>7376348</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>SCL.NZ</t>
+          <t>SDL.NZ</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Scales Corporation Limited Ordi</t>
+          <t>Solution Dynamics Limited Ordin</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>4.49</v>
+        <v>3.1</v>
       </c>
       <c r="E96" t="n">
-        <v>4.39</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
-        <v>0.137485</v>
+        <v>0.245378</v>
       </c>
       <c r="G96" t="n">
-        <v>2.63</v>
+        <v>0.367</v>
       </c>
       <c r="H96" t="n">
-        <v>637988608</v>
+        <v>45383380</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>SCT.NZ</t>
+          <t>SEK.NZ</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Scott Technology Limited Ordina</t>
+          <t>Seeka Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>2.91</v>
+        <v>5.25</v>
       </c>
       <c r="E97" t="n">
-        <v>2.92</v>
+        <v>5.23</v>
       </c>
       <c r="F97" t="n">
-        <v>0.7194160000000001</v>
+        <v>0.718767</v>
       </c>
       <c r="G97" t="n">
-        <v>1.198</v>
+        <v>5.985</v>
       </c>
       <c r="H97" t="n">
-        <v>227885024</v>
+        <v>170034896</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>SCY.NZ</t>
+          <t>SKC.NZ</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Smiths City Group Limited Ordin</t>
+          <t>SkyCity Entertainment Group Lim</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>0.14</v>
+        <v>3.33</v>
       </c>
       <c r="E98" t="n">
-        <v>0.14</v>
+        <v>3.27</v>
       </c>
       <c r="F98" t="n">
-        <v>1.147586</v>
+        <v>1.321135</v>
       </c>
       <c r="G98" t="n">
-        <v>0.697</v>
+        <v>2.069</v>
       </c>
       <c r="H98" t="n">
-        <v>7376348</v>
+        <v>2524469760</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>SDL.NZ</t>
+          <t>SKL.NZ</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Solution Dynamics Limited Ordin</t>
+          <t>Skellerup Holdings Limited Ordi</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>3</v>
+        <v>5.45</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>5.26</v>
       </c>
       <c r="F99" t="n">
-        <v>0.285072</v>
+        <v>0.524303</v>
       </c>
       <c r="G99" t="n">
-        <v>0.367</v>
+        <v>0.954</v>
       </c>
       <c r="H99" t="n">
-        <v>43919400</v>
+        <v>1064254144</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>SKC.NZ</t>
+          <t>SKO.NZ</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>SkyCity Entertainment Group Lim</t>
+          <t>Serko Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>3.09</v>
+        <v>8</v>
       </c>
       <c r="E100" t="n">
-        <v>3.03</v>
+        <v>8.02</v>
       </c>
       <c r="F100" t="n">
-        <v>1.297418</v>
+        <v>1.687602</v>
       </c>
       <c r="G100" t="n">
-        <v>2.069</v>
+        <v>0.604</v>
       </c>
       <c r="H100" t="n">
-        <v>2349033472</v>
+        <v>860800000</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>SKL.NZ</t>
+          <t>SKT.NZ</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Skellerup Holdings Limited Ordi</t>
+          <t xml:space="preserve">Sky Network Television Limited </t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>5.43</v>
+        <v>0.166</v>
       </c>
       <c r="E101" t="n">
-        <v>5.44</v>
+        <v>0.163</v>
       </c>
       <c r="F101" t="n">
-        <v>0.508978</v>
+        <v>0.9458259999999999</v>
       </c>
       <c r="G101" t="n">
-        <v>0.954</v>
+        <v>0.234</v>
       </c>
       <c r="H101" t="n">
-        <v>1060348672</v>
+        <v>289882464</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>SKO.NZ</t>
+          <t>SML.NZ</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Serko Limited Ordinary Shares</t>
+          <t>Synlait Milk Limited (NS) Ordin</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>7.75</v>
+        <v>3.23</v>
       </c>
       <c r="E102" t="n">
-        <v>7.95</v>
+        <v>3.28</v>
       </c>
       <c r="F102" t="n">
-        <v>1.653759</v>
+        <v>0.5129899999999999</v>
       </c>
       <c r="G102" t="n">
-        <v>0.962</v>
+        <v>3.798</v>
       </c>
       <c r="H102" t="n">
-        <v>836922496</v>
+        <v>706019840</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>SKT.NZ</t>
+          <t>SPG.NZ</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sky Network Television Limited </t>
+          <t>Stride Prop &amp; Stride Invest Mgm</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0.161</v>
+        <v>2.6</v>
       </c>
       <c r="E103" t="n">
-        <v>0.159</v>
+        <v>2.64</v>
       </c>
       <c r="F103" t="n">
-        <v>0.982042</v>
+        <v>0.660398</v>
       </c>
       <c r="G103" t="n">
-        <v>0.234</v>
+        <v>2.124</v>
       </c>
       <c r="H103" t="n">
-        <v>281151072</v>
+        <v>3691245824</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>SML.NZ</t>
+          <t>SPK.NZ</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Synlait Milk Limited (NS) Ordin</t>
+          <t>Spark New Zealand Limited Ordin</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>3.47</v>
+        <v>4.87</v>
       </c>
       <c r="E104" t="n">
-        <v>3.4</v>
+        <v>4.87</v>
       </c>
       <c r="F104" t="n">
-        <v>0.5123450000000001</v>
+        <v>0.248756</v>
       </c>
       <c r="G104" t="n">
-        <v>3.798</v>
+        <v>0.779</v>
       </c>
       <c r="H104" t="n">
-        <v>758479552</v>
+        <v>9092922368</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>SNC.NZ</t>
+          <t>SPN.NZ</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Southern Charter Financial Grou</t>
+          <t xml:space="preserve">South Port New Zealand Limited </t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>0.008</v>
+        <v>8.57</v>
       </c>
       <c r="E105" t="n">
-        <v>0.008</v>
+        <v>8.5</v>
       </c>
       <c r="F105" t="n">
-        <v>0.062912</v>
+        <v>0.286898</v>
       </c>
       <c r="G105" t="n">
-        <v>0.004</v>
+        <v>1.784</v>
       </c>
       <c r="H105" t="n">
-        <v>4119152</v>
+        <v>224833088</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>SPG.NZ</t>
+          <t>SPY.NZ</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Stride Prop &amp; Stride Invest Mgm</t>
+          <t>Smartpay Holdings Limited Ordin</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>2.59</v>
+        <v>0.76</v>
       </c>
       <c r="E106" t="n">
-        <v>2.6</v>
+        <v>0.75</v>
       </c>
       <c r="F106" t="n">
-        <v>0.65695</v>
+        <v>1.386954</v>
       </c>
       <c r="G106" t="n">
-        <v>2.124</v>
+        <v>0.119</v>
       </c>
       <c r="H106" t="n">
-        <v>3677048576</v>
+        <v>176403600</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>SPK.NZ</t>
+          <t>STU.NZ</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Spark New Zealand Limited Ordin</t>
+          <t>Steel &amp; Tube Holdings Limited O</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>4.825</v>
+        <v>1.13</v>
       </c>
       <c r="E107" t="n">
-        <v>4.805</v>
+        <v>1.13</v>
       </c>
       <c r="F107" t="n">
-        <v>0.180695</v>
+        <v>1.378109</v>
       </c>
       <c r="G107" t="n">
-        <v>0.805</v>
+        <v>1.115</v>
       </c>
       <c r="H107" t="n">
-        <v>9008902144</v>
+        <v>187577744</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SPN.NZ</t>
+          <t>SUM.NZ</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t xml:space="preserve">South Port New Zealand Limited </t>
+          <t>Summerset Group Holdings Limite</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>8.52</v>
+        <v>15.34</v>
       </c>
       <c r="E108" t="n">
-        <v>8.5</v>
+        <v>15.2</v>
       </c>
       <c r="F108" t="n">
-        <v>0.234006</v>
+        <v>0.808301</v>
       </c>
       <c r="G108" t="n">
-        <v>1.784</v>
+        <v>5.967</v>
       </c>
       <c r="H108" t="n">
-        <v>223521360</v>
+        <v>3519026688</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SPY.NZ</t>
+          <t>TEM.NZ</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Smartpay Holdings Limited Ordin</t>
+          <t xml:space="preserve">Templeton Emerging Markets Plc </t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>0.74</v>
+        <v>3.61</v>
       </c>
       <c r="E109" t="n">
-        <v>0.765</v>
+        <v>3.52</v>
       </c>
       <c r="F109" t="n">
-        <v>1.305836</v>
+        <v>0.761344</v>
       </c>
       <c r="G109" t="n">
-        <v>0.119</v>
+        <v>15.704</v>
       </c>
       <c r="H109" t="n">
-        <v>176330896</v>
+        <v>896030848</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>STU.NZ</t>
+          <t>TGG.NZ</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Steel &amp; Tube Holdings Limited O</t>
+          <t>T&amp;G Global Limited Ordinary Sha</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>1.13</v>
+        <v>2.98</v>
       </c>
       <c r="E110" t="n">
-        <v>1.12</v>
+        <v>2.98</v>
       </c>
       <c r="F110" t="n">
-        <v>1.353535</v>
+        <v>0.44168</v>
       </c>
       <c r="G110" t="n">
-        <v>1.115</v>
+        <v>4.134</v>
       </c>
       <c r="H110" t="n">
-        <v>187577744</v>
+        <v>365178144</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>SUM.NZ</t>
+          <t>THL.NZ</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Summerset Group Holdings Limite</t>
+          <t>Tourism Holdings Limited Ordina</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>13.76</v>
+        <v>2.44</v>
       </c>
       <c r="E111" t="n">
-        <v>13.2</v>
+        <v>2.33</v>
       </c>
       <c r="F111" t="n">
-        <v>0.76487</v>
+        <v>1.564145</v>
       </c>
       <c r="G111" t="n">
-        <v>5.967</v>
+        <v>2.191</v>
       </c>
       <c r="H111" t="n">
-        <v>3156571648</v>
+        <v>738914944</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>TCL.NZ</t>
+          <t>TLL.NZ</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>The City of London Investment T</t>
+          <t>TIL Logistics Group Ltd Ordinar</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>7.88</v>
+        <v>1.75</v>
       </c>
       <c r="E112" t="n">
-        <v>7.85</v>
+        <v>1.75</v>
       </c>
       <c r="F112" t="n">
-        <v>0.789001</v>
+        <v>0.75862</v>
       </c>
       <c r="G112" t="n">
-        <v>5.237</v>
+        <v>0.443</v>
       </c>
       <c r="H112" t="n">
-        <v>3525204736</v>
+        <v>153448576</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>TEM.NZ</t>
+          <t>TLT.NZ</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t xml:space="preserve">Templeton Emerging Markets Plc </t>
+          <t>Tilt Renewables Limited Ordinar</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>3.58</v>
+        <v>8.01</v>
       </c>
       <c r="E113" t="n">
-        <v>3.55</v>
+        <v>8.01</v>
       </c>
       <c r="F113" t="n">
-        <v>0.761344</v>
+        <v>0.590445</v>
       </c>
       <c r="G113" t="n">
-        <v>3.174</v>
+        <v>4.402</v>
       </c>
       <c r="H113" t="n">
-        <v>888584640</v>
+        <v>3021628416</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>TGG.NZ</t>
+          <t>TPW.NZ</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>T&amp;G Global Limited Ordinary Sha</t>
+          <t>Trustpower Limited Ordinary Sha</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>2.95</v>
+        <v>7.9</v>
       </c>
       <c r="E114" t="n">
-        <v>2.93</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="F114" t="n">
-        <v>0.388327</v>
+        <v>0.288736</v>
       </c>
       <c r="G114" t="n">
-        <v>4.208</v>
+        <v>3.418</v>
       </c>
       <c r="H114" t="n">
-        <v>361501856</v>
+        <v>2472486656</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>THL.NZ</t>
+          <t>TRA.NZ</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Tourism Holdings Limited Ordina</t>
+          <t>Turners Automotive Group Ltd Or</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>2.3</v>
+        <v>4.3</v>
       </c>
       <c r="E115" t="n">
-        <v>2.27</v>
+        <v>4.3</v>
       </c>
       <c r="F115" t="n">
-        <v>1.553872</v>
+        <v>1.092997</v>
       </c>
       <c r="G115" t="n">
-        <v>2.191</v>
+        <v>2.73</v>
       </c>
       <c r="H115" t="n">
-        <v>696518144</v>
+        <v>367885248</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>TPW.NZ</t>
+          <t>TRU.NZ</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Trustpower Limited Ordinary Sha</t>
+          <t>TruScreen Group Limited Ordinar</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>8.220000000000001</v>
+        <v>0.062</v>
       </c>
       <c r="E116" t="n">
-        <v>8.25</v>
+        <v>0.06</v>
       </c>
       <c r="F116" t="n">
-        <v>0.299836</v>
+        <v>0.491431</v>
       </c>
       <c r="G116" t="n">
-        <v>3.418</v>
+        <v>0.031</v>
       </c>
       <c r="H116" t="n">
-        <v>2572637952</v>
+        <v>22497690</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>TRA.NZ</t>
+          <t>TWR.NZ</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Turners Automotive Group Ltd Or</t>
+          <t>Tower Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>4.27</v>
+        <v>0.695</v>
       </c>
       <c r="E117" t="n">
-        <v>4.3</v>
+        <v>0.7</v>
       </c>
       <c r="F117" t="n">
-        <v>1.093714</v>
+        <v>0.387114</v>
       </c>
       <c r="G117" t="n">
-        <v>2.73</v>
+        <v>0.842</v>
       </c>
       <c r="H117" t="n">
-        <v>365273728</v>
+        <v>293044672</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>TRU.NZ</t>
+          <t>VCT.NZ</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>TruScreen Group Limited Ordinar</t>
+          <t>Vector Limited (NS) Ordinary Sh</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0.06</v>
+        <v>4.15</v>
       </c>
       <c r="E118" t="n">
-        <v>0.063</v>
+        <v>4.26</v>
       </c>
       <c r="F118" t="n">
-        <v>0.507856</v>
+        <v>0.410724</v>
       </c>
       <c r="G118" t="n">
-        <v>0.031</v>
+        <v>2.268</v>
       </c>
       <c r="H118" t="n">
-        <v>21771958</v>
+        <v>4150000128</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>TWR.NZ</t>
+          <t>VGL.NZ</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Tower Limited Ordinary Shares</t>
+          <t>Vista Group International Ltd O</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0.72</v>
+        <v>2.46</v>
       </c>
       <c r="E119" t="n">
-        <v>0.71</v>
+        <v>2.27</v>
       </c>
       <c r="F119" t="n">
-        <v>0.404601</v>
+        <v>1.693753</v>
       </c>
       <c r="G119" t="n">
-        <v>0.842</v>
+        <v>0.705</v>
       </c>
       <c r="H119" t="n">
-        <v>303585856</v>
+        <v>562884928</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>VCT.NZ</t>
+          <t>VHP.NZ</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Vector Limited (NS) Ordinary Sh</t>
+          <t>Vital Healthcare Property Trust</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>4.11</v>
+        <v>3.275</v>
       </c>
       <c r="E120" t="n">
-        <v>4.08</v>
+        <v>3.295</v>
       </c>
       <c r="F120" t="n">
-        <v>0.391694</v>
+        <v>0.412382</v>
       </c>
       <c r="G120" t="n">
-        <v>2.268</v>
+        <v>2.547</v>
       </c>
       <c r="H120" t="n">
-        <v>4110000128</v>
+        <v>1696299392</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>VGL.NZ</t>
+          <t>VTL.NZ</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Vista Group International Ltd O</t>
+          <t>Vital Limited Ordinary Shares</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>2.19</v>
+        <v>0.75</v>
       </c>
       <c r="E121" t="n">
-        <v>2.16</v>
+        <v>0.74</v>
       </c>
       <c r="F121" t="n">
-        <v>1.681257</v>
+        <v>0.342857</v>
       </c>
       <c r="G121" t="n">
-        <v>0.705</v>
+        <v>0.999</v>
       </c>
       <c r="H121" t="n">
-        <v>501104896</v>
+        <v>31035676</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>VHP.NZ</t>
+          <t>WBC.NZ</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Vital Healthcare Property Trust</t>
+          <t>Westpac Banking Corporation Ord</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>3.295</v>
+        <v>27.07</v>
       </c>
       <c r="E122" t="n">
-        <v>3.28</v>
+        <v>27.09</v>
       </c>
       <c r="F122" t="n">
-        <v>0.41863</v>
+        <v>0.762464</v>
       </c>
       <c r="G122" t="n">
-        <v>2.893</v>
+        <v>28.026</v>
       </c>
       <c r="H122" t="n">
-        <v>1712586112</v>
+        <v>99617054720</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>VTL.NZ</t>
+          <t>WDT.NZ</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Vital Limited Ordinary Shares</t>
+          <t>Wellington Drive Technologies L</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>0.75</v>
+        <v>0.123</v>
       </c>
       <c r="E123" t="n">
-        <v>0.75</v>
+        <v>0.127</v>
       </c>
       <c r="F123" t="n">
-        <v>0.32716</v>
+        <v>0.853221</v>
       </c>
       <c r="G123" t="n">
-        <v>0.999</v>
+        <v>0.034</v>
       </c>
       <c r="H123" t="n">
-        <v>31035676</v>
+        <v>53125548</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>WBC.NZ</t>
+          <t>WHS.NZ</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Westpac Banking Corporation Ord</t>
+          <t>The Warehouse Group Limited Ord</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>27</v>
+        <v>3.78</v>
       </c>
       <c r="E124" t="n">
-        <v>26.96</v>
+        <v>3.79</v>
       </c>
       <c r="F124" t="n">
-        <v>0.748035</v>
+        <v>0.312327</v>
       </c>
       <c r="G124" t="n">
-        <v>28.794</v>
+        <v>1.247</v>
       </c>
       <c r="H124" t="n">
-        <v>98965528576</v>
+        <v>1311066624</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>WDT.NZ</t>
+          <t>ZEL.NZ</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Wellington Drive Technologies L</t>
+          <t>Z Energy Limited Ordinary Share</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>0.115</v>
+        <v>3.52</v>
       </c>
       <c r="E125" t="n">
-        <v>0.115</v>
+        <v>3.52</v>
       </c>
       <c r="F125" t="n">
-        <v>0.920314</v>
+        <v>0.873389</v>
       </c>
       <c r="G125" t="n">
-        <v>0.034</v>
+        <v>1.948</v>
       </c>
       <c r="H125" t="n">
-        <v>49670228</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>WHS.NZ</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>The Warehouse Group Limited Ord</t>
-        </is>
-      </c>
-      <c r="D126" t="n">
-        <v>3.62</v>
-      </c>
-      <c r="E126" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="F126" t="n">
-        <v>0.329405</v>
-      </c>
-      <c r="G126" t="n">
-        <v>1.247</v>
-      </c>
-      <c r="H126" t="n">
-        <v>1255571712</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="n">
-        <v>171</v>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>ZEL.NZ</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Z Energy Limited Ordinary Share</t>
-        </is>
-      </c>
-      <c r="D127" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="E127" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="F127" t="n">
-        <v>0.859708</v>
-      </c>
-      <c r="G127" t="n">
-        <v>1.948</v>
-      </c>
-      <c r="H127" t="n">
-        <v>1804875392</v>
+        <v>1830882176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>